<commit_message>
The never ending cleanup process.
</commit_message>
<xml_diff>
--- a/data-raw/NutrientData/nutrientDetails/USDA GFS IMPACT V20.xlsx
+++ b/data-raw/NutrientData/nutrientDetails/USDA GFS IMPACT V20.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27217"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27224"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4360" yWindow="3140" windowWidth="28800" windowHeight="16420"/>
+    <workbookView xWindow="0" yWindow="540" windowWidth="28800" windowHeight="16420"/>
   </bookViews>
   <sheets>
     <sheet name="Reference" sheetId="1" r:id="rId1"/>
     <sheet name="Notes" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="150001" refMode="R1C1" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="355">
   <si>
     <t>Bananas</t>
   </si>
@@ -473,9 +473,6 @@
   </si>
   <si>
     <t>35% (skin and stems)</t>
-  </si>
-  <si>
-    <t>30% (bone)</t>
   </si>
   <si>
     <t>46% (hulls)</t>
@@ -1847,7 +1844,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
@@ -2236,6 +2233,9 @@
     </xf>
     <xf numFmtId="165" fontId="7" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="158">
@@ -2699,8 +2699,8 @@
   <dimension ref="A1:BL66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BL3" sqref="A3:XFD3"/>
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2780,7 +2780,7 @@
         <v>94</v>
       </c>
       <c r="O1" s="103" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="P1" s="37" t="s">
         <v>95</v>
@@ -2885,19 +2885,19 @@
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G2" s="88" t="s">
         <v>91</v>
       </c>
       <c r="H2" s="41" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>90</v>
       </c>
       <c r="J2" s="42" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K2" s="6"/>
       <c r="L2" s="43" t="s">
@@ -3001,196 +3001,196 @@
     </row>
     <row r="3" spans="1:64" s="18" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D3" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>240</v>
+      </c>
+      <c r="F3" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="E3" s="20" t="s">
-        <v>241</v>
-      </c>
-      <c r="F3" s="20" t="s">
+      <c r="G3" s="89" t="s">
         <v>144</v>
       </c>
-      <c r="G3" s="89" t="s">
+      <c r="H3" s="47" t="s">
         <v>145</v>
       </c>
-      <c r="H3" s="47" t="s">
+      <c r="I3" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="I3" s="20" t="s">
+      <c r="J3" s="47" t="s">
         <v>147</v>
       </c>
-      <c r="J3" s="47" t="s">
+      <c r="K3" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="K3" s="20" t="s">
-        <v>149</v>
-      </c>
       <c r="L3" s="48" t="s">
+        <v>169</v>
+      </c>
+      <c r="M3" s="44" t="s">
+        <v>188</v>
+      </c>
+      <c r="N3" s="44" t="s">
+        <v>189</v>
+      </c>
+      <c r="O3" s="104" t="s">
+        <v>187</v>
+      </c>
+      <c r="P3" s="44" t="s">
+        <v>190</v>
+      </c>
+      <c r="Q3" s="44" t="s">
+        <v>186</v>
+      </c>
+      <c r="R3" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="S3" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="T3" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="U3" s="45" t="s">
+        <v>194</v>
+      </c>
+      <c r="V3" s="44" t="s">
+        <v>195</v>
+      </c>
+      <c r="W3" s="46" t="s">
         <v>170</v>
       </c>
-      <c r="M3" s="44" t="s">
-        <v>189</v>
-      </c>
-      <c r="N3" s="44" t="s">
-        <v>190</v>
-      </c>
-      <c r="O3" s="104" t="s">
-        <v>188</v>
-      </c>
-      <c r="P3" s="44" t="s">
-        <v>191</v>
-      </c>
-      <c r="Q3" s="44" t="s">
-        <v>187</v>
-      </c>
-      <c r="R3" s="44" t="s">
-        <v>192</v>
-      </c>
-      <c r="S3" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="T3" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="U3" s="45" t="s">
-        <v>195</v>
-      </c>
-      <c r="V3" s="44" t="s">
+      <c r="X3" s="44" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y3" s="44" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z3" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="W3" s="46" t="s">
+      <c r="AA3" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB3" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="AC3" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="AD3" s="110" t="s">
+        <v>199</v>
+      </c>
+      <c r="AE3" s="44" t="s">
+        <v>177</v>
+      </c>
+      <c r="AF3" s="44" t="s">
+        <v>178</v>
+      </c>
+      <c r="AG3" s="44" t="s">
+        <v>209</v>
+      </c>
+      <c r="AH3" s="44" t="s">
+        <v>179</v>
+      </c>
+      <c r="AI3" s="44" t="s">
+        <v>176</v>
+      </c>
+      <c r="AJ3" s="44" t="s">
+        <v>180</v>
+      </c>
+      <c r="AK3" s="44" t="s">
+        <v>343</v>
+      </c>
+      <c r="AL3" s="44" t="s">
+        <v>181</v>
+      </c>
+      <c r="AM3" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="AN3" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="AO3" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="AP3" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="AQ3" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="AR3" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="AS3" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="AT3" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="AU3" s="18" t="s">
+        <v>318</v>
+      </c>
+      <c r="AV3" s="49" t="s">
+        <v>155</v>
+      </c>
+      <c r="AW3" s="49" t="s">
+        <v>172</v>
+      </c>
+      <c r="AX3" s="49" t="s">
+        <v>340</v>
+      </c>
+      <c r="AY3" s="49" t="s">
+        <v>173</v>
+      </c>
+      <c r="AZ3" s="49" t="s">
+        <v>174</v>
+      </c>
+      <c r="BA3" s="49" t="s">
+        <v>175</v>
+      </c>
+      <c r="BB3" s="49" t="s">
+        <v>202</v>
+      </c>
+      <c r="BC3" s="49" t="s">
+        <v>203</v>
+      </c>
+      <c r="BD3" s="49" t="s">
+        <v>342</v>
+      </c>
+      <c r="BE3" s="49" t="s">
+        <v>208</v>
+      </c>
+      <c r="BF3" s="49" t="s">
+        <v>204</v>
+      </c>
+      <c r="BG3" s="49" t="s">
+        <v>207</v>
+      </c>
+      <c r="BH3" s="49" t="s">
+        <v>205</v>
+      </c>
+      <c r="BI3" s="49" t="s">
+        <v>341</v>
+      </c>
+      <c r="BJ3" s="49" t="s">
+        <v>206</v>
+      </c>
+      <c r="BK3" s="49" t="s">
+        <v>344</v>
+      </c>
+      <c r="BL3" s="49" t="s">
         <v>171</v>
-      </c>
-      <c r="X3" s="44" t="s">
-        <v>322</v>
-      </c>
-      <c r="Y3" s="44" t="s">
-        <v>323</v>
-      </c>
-      <c r="Z3" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="AA3" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="AB3" s="9" t="s">
-        <v>198</v>
-      </c>
-      <c r="AC3" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="AD3" s="110" t="s">
-        <v>200</v>
-      </c>
-      <c r="AE3" s="44" t="s">
-        <v>178</v>
-      </c>
-      <c r="AF3" s="44" t="s">
-        <v>179</v>
-      </c>
-      <c r="AG3" s="44" t="s">
-        <v>210</v>
-      </c>
-      <c r="AH3" s="44" t="s">
-        <v>180</v>
-      </c>
-      <c r="AI3" s="44" t="s">
-        <v>177</v>
-      </c>
-      <c r="AJ3" s="44" t="s">
-        <v>181</v>
-      </c>
-      <c r="AK3" s="44" t="s">
-        <v>344</v>
-      </c>
-      <c r="AL3" s="44" t="s">
-        <v>182</v>
-      </c>
-      <c r="AM3" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="AN3" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="AO3" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="AP3" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="AQ3" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="AR3" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="AS3" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="AT3" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="AU3" s="18" t="s">
-        <v>319</v>
-      </c>
-      <c r="AV3" s="49" t="s">
-        <v>156</v>
-      </c>
-      <c r="AW3" s="49" t="s">
-        <v>173</v>
-      </c>
-      <c r="AX3" s="49" t="s">
-        <v>341</v>
-      </c>
-      <c r="AY3" s="49" t="s">
-        <v>174</v>
-      </c>
-      <c r="AZ3" s="49" t="s">
-        <v>175</v>
-      </c>
-      <c r="BA3" s="49" t="s">
-        <v>176</v>
-      </c>
-      <c r="BB3" s="49" t="s">
-        <v>203</v>
-      </c>
-      <c r="BC3" s="49" t="s">
-        <v>204</v>
-      </c>
-      <c r="BD3" s="49" t="s">
-        <v>343</v>
-      </c>
-      <c r="BE3" s="49" t="s">
-        <v>209</v>
-      </c>
-      <c r="BF3" s="49" t="s">
-        <v>205</v>
-      </c>
-      <c r="BG3" s="49" t="s">
-        <v>208</v>
-      </c>
-      <c r="BH3" s="49" t="s">
-        <v>206</v>
-      </c>
-      <c r="BI3" s="49" t="s">
-        <v>342</v>
-      </c>
-      <c r="BJ3" s="49" t="s">
-        <v>207</v>
-      </c>
-      <c r="BK3" s="49" t="s">
-        <v>345</v>
-      </c>
-      <c r="BL3" s="49" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:64" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -3222,16 +3222,16 @@
     </row>
     <row r="5" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A5" s="27" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E5" s="8"/>
       <c r="H5" s="16">
@@ -3333,7 +3333,7 @@
       </c>
       <c r="AU5" s="58"/>
       <c r="AV5" s="49" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AW5" s="49"/>
       <c r="AX5" s="49"/>
@@ -3354,16 +3354,16 @@
     </row>
     <row r="6" spans="1:64" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="27" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E6" s="8"/>
       <c r="H6" s="16">
@@ -3451,7 +3451,7 @@
       </c>
       <c r="AU6" s="58"/>
       <c r="AV6" s="49" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AW6" s="49"/>
       <c r="AX6" s="49"/>
@@ -3472,16 +3472,16 @@
     </row>
     <row r="7" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A7" s="27" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E7" s="8"/>
       <c r="H7" s="16">
@@ -3583,7 +3583,7 @@
       </c>
       <c r="AU7" s="58"/>
       <c r="AV7" s="49" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AW7" s="49"/>
       <c r="AX7" s="49"/>
@@ -3610,10 +3610,10 @@
         <v>37</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="8">
@@ -3718,7 +3718,7 @@
         <v>0</v>
       </c>
       <c r="AV8" s="49" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AW8" s="49"/>
       <c r="AX8" s="49"/>
@@ -3745,17 +3745,17 @@
         <v>38</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="8">
         <v>12101001</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H9" s="15">
         <v>100</v>
@@ -3856,7 +3856,7 @@
         <v>302</v>
       </c>
       <c r="AV9" s="49" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AW9" s="49">
         <v>0.8</v>
@@ -3915,17 +3915,17 @@
         <v>40</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E10" s="8"/>
       <c r="F10" s="8">
         <v>18101045</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H10" s="15">
         <v>100</v>
@@ -4029,7 +4029,7 @@
         <v>601</v>
       </c>
       <c r="AV10" s="49" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AW10" s="49">
         <v>0.55000000000000004</v>
@@ -4088,10 +4088,10 @@
         <v>42</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="8">
@@ -4199,7 +4199,7 @@
         <v>3454</v>
       </c>
       <c r="AV11" s="49" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AW11" s="49">
         <v>0.85</v>
@@ -4258,23 +4258,21 @@
         <v>58</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8">
         <v>18301073</v>
       </c>
       <c r="G12" s="90"/>
-      <c r="H12" s="16">
-        <v>70</v>
-      </c>
-      <c r="I12" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="J12" s="50">
+      <c r="H12" s="120">
+        <v>100</v>
+      </c>
+      <c r="I12" s="123"/>
+      <c r="J12" s="122">
         <v>61</v>
       </c>
       <c r="L12" s="43">
@@ -4369,7 +4367,7 @@
         <v>805</v>
       </c>
       <c r="AV12" s="49" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AW12" s="49">
         <v>0.7</v>
@@ -4428,10 +4426,10 @@
         <v>76</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E13" s="31"/>
       <c r="F13" s="31"/>
@@ -4535,7 +4533,7 @@
         <v>522</v>
       </c>
       <c r="AV13" s="49" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AW13" s="49">
         <v>0.65</v>
@@ -4594,10 +4592,10 @@
         <v>43</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="8">
@@ -4700,7 +4698,7 @@
         <v>230</v>
       </c>
       <c r="AV14" s="49" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AW14" s="49"/>
       <c r="AX14" s="49"/>
@@ -4727,10 +4725,10 @@
         <v>41</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="8">
@@ -4741,7 +4739,7 @@
         <v>38.4</v>
       </c>
       <c r="I15" s="21" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="J15" s="50"/>
       <c r="L15" s="43">
@@ -4835,7 +4833,7 @@
         <v>3142</v>
       </c>
       <c r="AV15" s="49" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AW15" s="49"/>
       <c r="AX15" s="49"/>
@@ -4862,10 +4860,10 @@
         <v>48</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E16" s="31"/>
       <c r="F16" s="24">
@@ -4972,7 +4970,7 @@
         <v>302</v>
       </c>
       <c r="AV16" s="49" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AW16" s="49">
         <v>0.8</v>
@@ -5031,10 +5029,10 @@
         <v>78</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E17" s="31"/>
       <c r="F17" s="61"/>
@@ -5127,7 +5125,7 @@
         <v>522</v>
       </c>
       <c r="AV17" s="49" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AW17" s="49">
         <v>0.65</v>
@@ -5180,16 +5178,16 @@
     </row>
     <row r="18" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E18" s="8"/>
       <c r="F18" s="23"/>
@@ -5197,7 +5195,7 @@
         <v>87</v>
       </c>
       <c r="I18" s="62" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L18" s="48">
         <v>83.01</v>
@@ -5297,7 +5295,7 @@
         <v>2753</v>
       </c>
       <c r="AV18" s="49" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AW18" s="49">
         <v>0.9</v>
@@ -5356,10 +5354,10 @@
         <v>44</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8">
@@ -5475,7 +5473,7 @@
         <v>105</v>
       </c>
       <c r="AV19" s="49" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AW19" s="49">
         <v>0.85</v>
@@ -5528,16 +5526,16 @@
     </row>
     <row r="20" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E20" s="8"/>
       <c r="F20" s="23"/>
@@ -5627,7 +5625,7 @@
         <v>710</v>
       </c>
       <c r="AV20" s="49" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AW20" s="49"/>
       <c r="AX20" s="49"/>
@@ -5648,16 +5646,16 @@
     </row>
     <row r="21" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E21" s="8"/>
       <c r="H21" s="16">
@@ -5746,7 +5744,7 @@
         <v>2455</v>
       </c>
       <c r="AV21" s="49" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AW21" s="49">
         <v>0.95</v>
@@ -5799,16 +5797,16 @@
     </row>
     <row r="22" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
@@ -5899,7 +5897,7 @@
         <v>2305</v>
       </c>
       <c r="AV22" s="49" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="AW22" s="49">
         <v>0.9</v>
@@ -5958,10 +5956,10 @@
         <v>79</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E23" s="8"/>
       <c r="F23" s="8">
@@ -6067,7 +6065,7 @@
         <v>502</v>
       </c>
       <c r="AV23" s="49" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="AW23" s="49">
         <v>0.7</v>
@@ -6126,10 +6124,10 @@
         <v>49</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E24" s="8"/>
       <c r="F24" s="8">
@@ -6221,7 +6219,7 @@
         <v>14</v>
       </c>
       <c r="AV24" s="49" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AW24" s="49"/>
       <c r="AX24" s="49"/>
@@ -6248,10 +6246,10 @@
         <v>50</v>
       </c>
       <c r="C25" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="D25" s="8" t="s">
         <v>267</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>268</v>
       </c>
       <c r="E25" s="8"/>
       <c r="F25" s="8">
@@ -6352,7 +6350,7 @@
         <v>302</v>
       </c>
       <c r="AV25" s="49" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AW25" s="49">
         <v>0.8</v>
@@ -6411,10 +6409,10 @@
         <v>55</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E26" s="8"/>
       <c r="F26" s="8">
@@ -6518,7 +6516,7 @@
         <v>5019</v>
       </c>
       <c r="AV26" s="49" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="AW26" s="49">
         <v>1</v>
@@ -6577,10 +6575,10 @@
         <v>45</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E27" s="8"/>
       <c r="F27" s="8">
@@ -6686,7 +6684,7 @@
         <v>5019</v>
       </c>
       <c r="AV27" s="49" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="AW27" s="49">
         <v>1</v>
@@ -6745,10 +6743,10 @@
         <v>60</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E28" s="8"/>
       <c r="F28" s="8">
@@ -6857,7 +6855,7 @@
         <v>5019</v>
       </c>
       <c r="AV28" s="49" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="AW28" s="49">
         <v>1</v>
@@ -6916,10 +6914,10 @@
         <v>61</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E29" s="8"/>
       <c r="F29" s="8">
@@ -7025,7 +7023,7 @@
         <v>5019</v>
       </c>
       <c r="AV29" s="49" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="AW29" s="49">
         <v>1</v>
@@ -7078,16 +7076,16 @@
     </row>
     <row r="30" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>46</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E30" s="8"/>
       <c r="F30" s="8">
@@ -7193,7 +7191,7 @@
         <v>2202</v>
       </c>
       <c r="AV30" s="49" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="AW30" s="49">
         <v>0.85</v>
@@ -7252,10 +7250,10 @@
         <v>84</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D31" s="31" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E31" s="31"/>
       <c r="F31" s="31"/>
@@ -7348,7 +7346,7 @@
         <v>522</v>
       </c>
       <c r="AV31" s="49" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AW31" s="49">
         <v>0.65</v>
@@ -7407,10 +7405,10 @@
         <v>74</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D32" s="31" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E32" s="31"/>
       <c r="F32" s="65"/>
@@ -7516,7 +7514,7 @@
         <v>153</v>
       </c>
       <c r="AV32" s="49" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="AW32" s="49">
         <v>0.8</v>
@@ -7575,17 +7573,17 @@
         <v>56</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E33" s="8"/>
       <c r="F33" s="8">
         <v>18103095</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H33" s="16">
         <v>100</v>
@@ -7677,7 +7675,7 @@
         <v>1254</v>
       </c>
       <c r="AV33" s="49" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AW33" s="49">
         <v>0.6</v>
@@ -7736,10 +7734,10 @@
         <v>57</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E34" s="8"/>
       <c r="F34" s="8">
@@ -7847,7 +7845,7 @@
         <v>3308</v>
       </c>
       <c r="AV34" s="49" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="AW34" s="49">
         <v>0.8</v>
@@ -7906,10 +7904,10 @@
         <v>59</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E35" s="8"/>
       <c r="F35" s="8">
@@ -8015,7 +8013,7 @@
         <v>432</v>
       </c>
       <c r="AV35" s="49" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AW35" s="49">
         <v>0.8</v>
@@ -8074,10 +8072,10 @@
         <v>62</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E36" s="8"/>
       <c r="F36" s="8">
@@ -8088,7 +8086,7 @@
         <v>54</v>
       </c>
       <c r="I36" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J36" s="50"/>
       <c r="L36" s="43">
@@ -8182,7 +8180,7 @@
         <v>0</v>
       </c>
       <c r="AV36" s="49" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AW36" s="49"/>
       <c r="AX36" s="49"/>
@@ -8209,10 +8207,10 @@
         <v>63</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D37" s="31" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E37" s="31"/>
       <c r="F37" s="31"/>
@@ -8313,7 +8311,7 @@
         <v>302</v>
       </c>
       <c r="AV37" s="49" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AW37" s="49">
         <v>0.8</v>
@@ -8372,10 +8370,10 @@
         <v>72</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E38" s="8"/>
       <c r="F38" s="8">
@@ -8481,7 +8479,7 @@
         <v>522</v>
       </c>
       <c r="AV38" s="49" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AW38" s="49">
         <v>0.65</v>
@@ -8534,16 +8532,16 @@
     </row>
     <row r="39" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B39" s="9" t="s">
         <v>71</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E39" s="8"/>
       <c r="F39" s="8">
@@ -8648,7 +8646,7 @@
         <v>0</v>
       </c>
       <c r="AV39" s="49" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AW39" s="49"/>
       <c r="AX39" s="49"/>
@@ -8675,23 +8673,23 @@
         <v>64</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E40" s="8"/>
       <c r="F40" s="8">
         <v>24302043</v>
       </c>
       <c r="G40" s="92" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="H40" s="16">
         <v>72</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J40" s="50"/>
       <c r="L40" s="43">
@@ -8788,7 +8786,7 @@
         <v>3708</v>
       </c>
       <c r="AV40" s="49" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AW40" s="49">
         <v>0.8</v>
@@ -8847,10 +8845,10 @@
         <v>81</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E41" s="8"/>
       <c r="F41" s="31"/>
@@ -8859,7 +8857,7 @@
         <v>86</v>
       </c>
       <c r="I41" s="31" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="J41" s="59"/>
       <c r="L41" s="43">
@@ -8963,7 +8961,7 @@
         <v>3454</v>
       </c>
       <c r="AV41" s="49" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AW41" s="49">
         <v>0.85</v>
@@ -9022,10 +9020,10 @@
         <v>66</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E42" s="8"/>
       <c r="F42" s="8">
@@ -9131,7 +9129,7 @@
         <v>5019</v>
       </c>
       <c r="AV42" s="49" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="AW42" s="49">
         <v>1</v>
@@ -9190,14 +9188,14 @@
         <v>65</v>
       </c>
       <c r="D43" s="31" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E43" s="31"/>
       <c r="F43" s="24">
         <v>11101001</v>
       </c>
       <c r="G43" s="33" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H43" s="16"/>
       <c r="I43" s="31"/>
@@ -9290,7 +9288,7 @@
         <v>0</v>
       </c>
       <c r="AV43" s="49" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AW43" s="49"/>
       <c r="AX43" s="49"/>
@@ -9317,10 +9315,10 @@
         <v>54</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D44" s="31" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E44" s="31"/>
       <c r="F44" s="31"/>
@@ -9424,7 +9422,7 @@
         <v>5019</v>
       </c>
       <c r="AV44" s="49" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="AW44" s="49">
         <v>1</v>
@@ -9483,10 +9481,10 @@
         <v>69</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E45" s="8"/>
       <c r="F45" s="8">
@@ -9580,7 +9578,7 @@
         <v>302</v>
       </c>
       <c r="AV45" s="49" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AW45" s="49">
         <v>0.8</v>
@@ -9639,10 +9637,10 @@
         <v>53</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E46" s="8"/>
       <c r="F46" s="8">
@@ -9653,7 +9651,7 @@
         <v>86</v>
       </c>
       <c r="I46" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J46" s="50"/>
       <c r="L46" s="43">
@@ -9750,7 +9748,7 @@
         <v>3708</v>
       </c>
       <c r="AV46" s="49" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AW46" s="49">
         <v>0.8</v>
@@ -9918,7 +9916,7 @@
         <v>522</v>
       </c>
       <c r="AV47" s="80" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AW47" s="80">
         <v>0.65</v>
@@ -9971,16 +9969,16 @@
     </row>
     <row r="48" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A48" s="27" t="s">
+        <v>336</v>
+      </c>
+      <c r="B48" s="28" t="s">
         <v>337</v>
       </c>
-      <c r="B48" s="28" t="s">
-        <v>338</v>
-      </c>
       <c r="C48" s="12" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H48" s="16">
         <v>100</v>
@@ -10087,7 +10085,7 @@
         <v>601</v>
       </c>
       <c r="AV48" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AW48" s="6">
         <v>0.55000000000000004</v>
@@ -10140,16 +10138,16 @@
     </row>
     <row r="49" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A49" s="27" t="s">
+        <v>338</v>
+      </c>
+      <c r="B49" s="28" t="s">
         <v>339</v>
       </c>
-      <c r="B49" s="28" t="s">
-        <v>340</v>
-      </c>
       <c r="C49" s="12" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="H49" s="70">
         <v>84.61767667588596</v>
@@ -10257,7 +10255,7 @@
         <v>3771</v>
       </c>
       <c r="AV49" s="68" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="AW49" s="68">
         <v>0.9</v>
@@ -10317,7 +10315,7 @@
       </c>
       <c r="C50" s="14"/>
       <c r="D50" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E50" s="8" t="s">
         <v>39</v>
@@ -10383,14 +10381,14 @@
     </row>
     <row r="51" spans="1:64" s="7" customFormat="1" ht="62" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B51" s="36" t="s">
         <v>47</v>
       </c>
       <c r="C51" s="95"/>
       <c r="D51" s="90" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E51" s="90" t="s">
         <v>47</v>
@@ -10399,7 +10397,7 @@
         <v>18102056</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H51" s="15"/>
       <c r="I51" s="5"/>
@@ -10464,7 +10462,7 @@
         <v>51</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E52" s="31" t="s">
         <v>51</v>
@@ -10532,7 +10530,7 @@
         <v>52</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E53" s="31" t="s">
         <v>52</v>
@@ -10601,7 +10599,7 @@
       </c>
       <c r="C54" s="12"/>
       <c r="D54" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E54" s="31" t="s">
         <v>82</v>
@@ -10674,7 +10672,7 @@
         <v>73</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E55" s="8" t="s">
         <v>73</v>
@@ -10744,7 +10742,7 @@
       </c>
       <c r="C56" s="22"/>
       <c r="D56" s="90" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E56" s="90" t="s">
         <v>88</v>
@@ -10815,7 +10813,7 @@
       </c>
       <c r="C57" s="14"/>
       <c r="D57" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E57" s="31" t="s">
         <v>70</v>
@@ -10884,7 +10882,7 @@
         <v>67</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E58" s="33" t="s">
         <v>67</v>
@@ -10954,7 +10952,7 @@
       </c>
       <c r="C59" s="14"/>
       <c r="D59" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E59" s="31" t="s">
         <v>68</v>
@@ -11008,17 +11006,17 @@
     </row>
     <row r="60" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A60" s="8" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C60" s="14"/>
       <c r="D60" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H60" s="16"/>
       <c r="O60" s="87"/>
@@ -11065,17 +11063,17 @@
     </row>
     <row r="61" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A61" s="8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C61" s="14"/>
       <c r="D61" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H61" s="16"/>
       <c r="O61" s="87"/>
@@ -11122,17 +11120,17 @@
     </row>
     <row r="62" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A62" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C62" s="14"/>
       <c r="D62" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H62" s="16"/>
       <c r="O62" s="87"/>
@@ -11179,17 +11177,17 @@
     </row>
     <row r="63" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A63" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C63" s="14"/>
       <c r="D63" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H63" s="16"/>
       <c r="O63" s="87"/>
@@ -11236,17 +11234,17 @@
     </row>
     <row r="64" spans="1:64" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C64" s="14"/>
       <c r="D64" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E64" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H64" s="16"/>
       <c r="O64" s="87"/>
@@ -11293,17 +11291,17 @@
     </row>
     <row r="65" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A65" s="8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C65" s="14"/>
       <c r="D65" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E65" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H65" s="16"/>
       <c r="L65" s="85"/>
@@ -11419,7 +11417,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="119" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Code changes to prepare for use of shiny
</commit_message>
<xml_diff>
--- a/data-raw/NutrientData/nutrientDetails/USDA GFS IMPACT V20.xlsx
+++ b/data-raw/NutrientData/nutrientDetails/USDA GFS IMPACT V20.xlsx
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="358">
   <si>
     <t>Bananas</t>
   </si>
@@ -1140,6 +1140,15 @@
   </si>
   <si>
     <t>see notes worksheet</t>
+  </si>
+  <si>
+    <t>47% ethanol</t>
+  </si>
+  <si>
+    <t>assume 4 % ethanol</t>
+  </si>
+  <si>
+    <t>assume 12% ethanol</t>
   </si>
 </sst>
 </file>
@@ -2699,13 +2708,13 @@
   <dimension ref="A1:BL66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E33" sqref="E33"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="21.1640625" style="6" customWidth="1"/>
     <col min="2" max="2" width="6.83203125" style="6" customWidth="1"/>
     <col min="3" max="3" width="6" style="12" customWidth="1"/>
     <col min="4" max="4" width="30.5" style="6" customWidth="1"/>
@@ -3220,7 +3229,7 @@
       <c r="AL4" s="52"/>
       <c r="AU4" s="53"/>
     </row>
-    <row r="5" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:64" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" s="27" t="s">
         <v>228</v>
       </c>
@@ -3234,6 +3243,9 @@
         <v>311</v>
       </c>
       <c r="E5" s="8"/>
+      <c r="G5" s="7" t="s">
+        <v>356</v>
+      </c>
       <c r="H5" s="16">
         <v>100</v>
       </c>
@@ -3366,6 +3378,9 @@
         <v>315</v>
       </c>
       <c r="E6" s="8"/>
+      <c r="G6" s="7" t="s">
+        <v>355</v>
+      </c>
       <c r="H6" s="16">
         <v>100</v>
       </c>
@@ -3470,7 +3485,7 @@
       <c r="BK6" s="49"/>
       <c r="BL6" s="49"/>
     </row>
-    <row r="7" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:64" ht="30" x14ac:dyDescent="0.2">
       <c r="A7" s="27" t="s">
         <v>229</v>
       </c>
@@ -3484,6 +3499,9 @@
         <v>313</v>
       </c>
       <c r="E7" s="8"/>
+      <c r="G7" s="7" t="s">
+        <v>357</v>
+      </c>
       <c r="H7" s="16">
         <v>100</v>
       </c>

</xml_diff>